<commit_message>
Add Project6_Report_Sprint2 and output file
</commit_message>
<xml_diff>
--- a/Team02Report.xlsx
+++ b/Team02Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SIT 19Fall Classes\CSS-555\Project\Project04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SIT 19Fall Classes\CSS-555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F50A02E-B362-48B5-913D-1611098D8E7C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1423FA54-655A-44CC-B455-166558180D7A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="294">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -164,9 +164,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Avoid:</t>
-  </si>
-  <si>
     <t>GitHub Username</t>
   </si>
   <si>
@@ -290,9 +287,6 @@
     <t>Siblings spacing</t>
   </si>
   <si>
-    <t>Fewer than 15 siblings</t>
-  </si>
-  <si>
     <t>Male last names</t>
   </si>
   <si>
@@ -308,9 +302,6 @@
     <t>Aunts and uncles</t>
   </si>
   <si>
-    <t>Correct gender for role</t>
-  </si>
-  <si>
     <t>Husband in family should be male and wife in family should be female</t>
   </si>
   <si>
@@ -326,31 +317,13 @@
     <t>List deceased</t>
   </si>
   <si>
-    <t>List living married</t>
-  </si>
-  <si>
-    <t>List living single</t>
-  </si>
-  <si>
     <t>List multiple births</t>
   </si>
   <si>
     <t>List orphans</t>
   </si>
   <si>
-    <t>List recent births</t>
-  </si>
-  <si>
-    <t>List recent deaths</t>
-  </si>
-  <si>
     <t>List recent survivors</t>
-  </si>
-  <si>
-    <t>List upcoming birthdays</t>
-  </si>
-  <si>
-    <t>List upcoming anniversaries</t>
   </si>
   <si>
     <t>Include input line numbers</t>
@@ -813,10 +786,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Undo</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Less group working time</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -942,10 +911,6 @@
   </si>
   <si>
     <t>Unique families by spouses</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unique families by spouses</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -990,6 +955,154 @@
   </si>
   <si>
     <t>13</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>10/20/2019</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Review Results:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Keep doing:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avoid:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Undo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US21</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US35</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US36</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US39</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US30</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US31</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US15</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US38</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Correct gender for role</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Correct gender for role</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>List recent births</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>List recent births</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>List recent deaths</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>List recent deaths</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>List upcoming anniversaries</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>List upcoming anniversaries</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>List living married</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>List living married</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>List living single</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>List living single</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>List upcoming birthdays</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>List upcoming birthdays</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fewer than 15 siblings</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fewer than 15 siblings</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fz</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>zh</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unique family by spouses</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">In this sprint, we have implemented all eight stories as we planned. Now, the program will report the error for the person whose birth  is after parents' death, the duplicate IDs, the duplicate name and birthday, the person whose marriage is before 14, the duplicate first names in a single family and check the spouses has a unique family. The code now can trace the line number and get rid off the invalid incomes while reading the gedcom file. The user story USC01 has similar functionality as US40. However, we do refactoring the object constructor attributes and variables to achieve a better perofomance of reading method.  </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Refactoring the code to eliminate bad smells. Efficient and effective team communication. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">When we implemented some stories, some additional functions which should be retreated as exclusive stories had been added. We need to better plan our stories to avoid achieving extra stories in a single story implement. </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1146,7 +1259,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1208,6 +1321,13 @@
     </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1394,7 +1514,7 @@
                   <c:v>42285</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42299</c:v>
+                  <c:v>42296</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>42313</c:v>
@@ -1530,6 +1650,9 @@
                 <c:pt idx="1">
                   <c:v>42285</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>42296</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1544,6 +1667,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2020,7 +2146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -2046,83 +2172,83 @@
         <v>22</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D5" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>161</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="14" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2143,10 +2269,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2180,16 +2306,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2197,16 +2323,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2214,16 +2340,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2231,16 +2357,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>210</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2248,16 +2374,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2265,16 +2391,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>216</v>
-      </c>
       <c r="D7" s="12" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2282,16 +2408,16 @@
         <v>1</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>217</v>
-      </c>
       <c r="D8" s="12" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2299,16 +2425,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>218</v>
-      </c>
       <c r="D9" s="12" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2316,16 +2442,16 @@
         <v>2</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2333,16 +2459,16 @@
         <v>2</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2350,16 +2476,16 @@
         <v>2</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2367,16 +2493,16 @@
         <v>2</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2384,16 +2510,16 @@
         <v>2</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -2401,16 +2527,16 @@
         <v>2</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2418,16 +2544,16 @@
         <v>2</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -2435,16 +2561,152 @@
         <v>2</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="C17" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>262</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>223</v>
+      <c r="C18" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -2458,8 +2720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2475,7 +2737,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2498,7 +2760,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B2" s="11">
         <v>42271</v>
@@ -2518,7 +2780,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B3" s="11">
         <v>42285</v>
@@ -2542,10 +2804,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B4" s="11">
-        <v>42299</v>
+        <v>42296</v>
       </c>
       <c r="C4">
         <v>16</v>
@@ -2553,10 +2815,21 @@
       <c r="D4">
         <v>8</v>
       </c>
+      <c r="E4" s="12">
+        <f>252+E3</f>
+        <v>712</v>
+      </c>
+      <c r="F4" s="8">
+        <v>270</v>
+      </c>
+      <c r="G4">
+        <f>(E4-E3)/F4*60</f>
+        <v>56</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B5" s="11">
         <v>42313</v>
@@ -2570,7 +2843,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B6" s="16">
         <v>42327</v>
@@ -2592,10 +2865,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2669,6 +2942,26 @@
         <v>138</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>42296</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>712</v>
+      </c>
+      <c r="E4">
+        <v>270</v>
+      </c>
+      <c r="F4" s="8">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2681,8 +2974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2724,7 +3017,7 @@
         <v>16</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="J1" s="18" t="s">
         <v>17</v>
@@ -2732,16 +3025,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E2" s="24">
         <v>15</v>
@@ -2756,24 +3049,24 @@
         <v>30</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E3" s="24">
         <v>20</v>
@@ -2791,21 +3084,21 @@
         <v>5</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E4" s="24">
         <v>20</v>
@@ -2823,21 +3116,21 @@
         <v>5</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E5" s="24">
         <v>20</v>
@@ -2855,21 +3148,21 @@
         <v>5</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E6" s="24">
         <v>20</v>
@@ -2887,21 +3180,21 @@
         <v>5</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E7" s="24">
         <v>20</v>
@@ -2919,21 +3212,21 @@
         <v>5</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E8" s="24">
         <v>10</v>
@@ -2948,24 +3241,24 @@
         <v>30</v>
       </c>
       <c r="I8" s="28" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E9" s="24">
         <v>25</v>
@@ -2983,17 +3276,17 @@
         <v>5</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="26" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="153" x14ac:dyDescent="0.2">
       <c r="B13" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -3004,37 +3297,37 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="26" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B17" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="15" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="5" t="s">
-        <v>30</v>
+      <c r="B20" s="26" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="15" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -3046,15 +3339,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="26.625" customWidth="1"/>
+    <col min="1" max="1" width="7.875" customWidth="1"/>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
     <col min="5" max="5" width="8.25" customWidth="1"/>
     <col min="6" max="7" width="9.125" customWidth="1"/>
     <col min="8" max="8" width="9.875" customWidth="1"/>
@@ -3088,24 +3382,24 @@
         <v>16</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="E2">
         <v>25</v>
@@ -3113,22 +3407,31 @@
       <c r="F2">
         <v>30</v>
       </c>
+      <c r="G2">
+        <v>42</v>
+      </c>
+      <c r="H2">
+        <v>40</v>
+      </c>
       <c r="I2" s="30" t="s">
-        <v>264</v>
+        <v>253</v>
+      </c>
+      <c r="J2" s="31" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="E3">
         <v>30</v>
@@ -3136,22 +3439,31 @@
       <c r="F3">
         <v>30</v>
       </c>
+      <c r="G3">
+        <v>30</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
       <c r="I3" s="30" t="s">
-        <v>264</v>
+        <v>253</v>
+      </c>
+      <c r="J3" s="31" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -3159,22 +3471,31 @@
       <c r="F4">
         <v>30</v>
       </c>
+      <c r="G4">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
       <c r="I4" s="30" t="s">
-        <v>264</v>
+        <v>253</v>
+      </c>
+      <c r="J4" s="31" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="E5">
         <v>30</v>
@@ -3182,22 +3503,31 @@
       <c r="F5">
         <v>30</v>
       </c>
+      <c r="G5">
+        <v>16</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
       <c r="I5" s="30" t="s">
-        <v>264</v>
+        <v>253</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="E6">
         <v>25</v>
@@ -3205,22 +3535,31 @@
       <c r="F6">
         <v>30</v>
       </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
+      </c>
       <c r="I6" s="30" t="s">
-        <v>264</v>
+        <v>253</v>
+      </c>
+      <c r="J6" s="31" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="E7">
         <v>30</v>
@@ -3228,22 +3567,31 @@
       <c r="F7">
         <v>30</v>
       </c>
+      <c r="G7">
+        <v>29</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
       <c r="I7" s="30" t="s">
-        <v>264</v>
+        <v>253</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="E8">
         <v>200</v>
@@ -3251,22 +3599,31 @@
       <c r="F8">
         <v>120</v>
       </c>
+      <c r="G8">
+        <v>60</v>
+      </c>
+      <c r="H8">
+        <v>40</v>
+      </c>
       <c r="I8" s="30" t="s">
-        <v>267</v>
+        <v>256</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="E9">
         <v>50</v>
@@ -3274,26 +3631,68 @@
       <c r="F9">
         <v>60</v>
       </c>
+      <c r="G9">
+        <v>40</v>
+      </c>
+      <c r="H9">
+        <v>50</v>
+      </c>
       <c r="I9" s="30" t="s">
-        <v>263</v>
+        <v>252</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="267.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="32" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B19" s="33" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="B23" s="33" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A2" sqref="A2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
@@ -3324,9 +3723,170 @@
         <v>17</v>
       </c>
     </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3379,8 +3939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3391,497 +3951,497 @@
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B15" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>113</v>
-      </c>
-      <c r="B16" t="s">
-        <v>72</v>
+        <v>104</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>284</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>119</v>
-      </c>
-      <c r="B22" t="s">
-        <v>78</v>
+        <v>110</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>270</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>255</v>
+        <v>290</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>128</v>
-      </c>
-      <c r="B31" t="s">
-        <v>84</v>
+        <v>119</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>278</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>129</v>
-      </c>
-      <c r="B32" t="s">
-        <v>85</v>
+        <v>120</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>280</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B35" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>133</v>
-      </c>
-      <c r="B36" t="s">
-        <v>88</v>
+        <v>124</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>272</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>134</v>
-      </c>
-      <c r="B37" t="s">
-        <v>89</v>
+        <v>125</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>274</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B38" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>136</v>
-      </c>
-      <c r="B39" t="s">
-        <v>91</v>
+        <v>127</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>282</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>137</v>
-      </c>
-      <c r="B40" t="s">
-        <v>92</v>
+        <v>128</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>276</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B41" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B42" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>